<commit_message>
analyse the first batch
</commit_message>
<xml_diff>
--- a/ParameterNameList/parameterList_task_DSST.xlsx
+++ b/ParameterNameList/parameterList_task_DSST.xlsx
@@ -5,17 +5,16 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\GitHub\Masud_OxfordCognition\Project03_Plasma_AD\OxCog_analysis_Plasma\ParameterNameList\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\GitHub\Masud_OxfordCognition\Project13_ECT\OxCog_analysis_ECT\ParameterNameList\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{29ED770B-FD4F-47F7-A477-B37DFB80DD5A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{92F9AF4A-A574-4519-8730-C5EED8360985}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="2256" windowWidth="25068" windowHeight="11556" activeTab="1" xr2:uid="{89D9FAA3-7342-4980-AE9A-5347263E0025}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="30936" windowHeight="16776" xr2:uid="{89D9FAA3-7342-4980-AE9A-5347263E0025}"/>
   </bookViews>
   <sheets>
-    <sheet name="key" sheetId="4" r:id="rId1"/>
+    <sheet name="all (2)" sheetId="6" r:id="rId1"/>
     <sheet name="all" sheetId="3" r:id="rId2"/>
-    <sheet name="all (2)" sheetId="5" r:id="rId3"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -36,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="39" uniqueCount="15">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="23" uniqueCount="14">
   <si>
     <t>plist</t>
   </si>
@@ -44,9 +43,6 @@
     <t>nlist</t>
   </si>
   <si>
-    <t>DSST_testTime</t>
-  </si>
-  <si>
     <t>DSST_nCorrectResponse</t>
   </si>
   <si>
@@ -80,7 +76,7 @@
     <t>time</t>
   </si>
   <si>
-    <t>testTime_DSST</t>
+    <t>testTime_dsst</t>
   </si>
 </sst>
 </file>
@@ -431,39 +427,49 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5C6A5F0B-1065-4194-BF87-FC2128B05854}">
-  <dimension ref="A1:C2"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2964E716-3BF0-45A2-AE80-B71C07197309}">
+  <dimension ref="A1:B4"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A2" sqref="A2:XFD2"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A3" sqref="A3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.77734375" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="34.44140625" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="44.33203125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="24.77734375" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="35.77734375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>0</v>
       </c>
       <c r="B1" t="s">
-        <v>1</v>
-      </c>
-      <c r="C1" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A2" t="s">
+        <v>13</v>
+      </c>
+      <c r="B2" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A3" t="s">
+        <v>2</v>
+      </c>
+      <c r="B3" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A2" t="s">
-        <v>3</v>
-      </c>
-      <c r="B2" t="s">
-        <v>7</v>
-      </c>
-      <c r="C2" t="s">
-        <v>12</v>
+    <row r="4" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A4" t="s">
+        <v>4</v>
+      </c>
+      <c r="B4" t="s">
+        <v>11</v>
       </c>
     </row>
   </sheetData>
@@ -475,8 +481,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{57EC45A0-751D-429E-9211-6A1DA8931C9E}">
   <dimension ref="A1:C5"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A12" sqref="A12"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A4" sqref="A4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.77734375" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -494,93 +500,18 @@
         <v>1</v>
       </c>
       <c r="C1" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="B2" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="C2" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A3" t="s">
-        <v>4</v>
-      </c>
-      <c r="B3" t="s">
-        <v>8</v>
-      </c>
-      <c r="C3" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A4" t="s">
-        <v>5</v>
-      </c>
-      <c r="B4" t="s">
-        <v>9</v>
-      </c>
-      <c r="C4" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A5" t="s">
-        <v>6</v>
-      </c>
-      <c r="B5" t="s">
-        <v>10</v>
-      </c>
-      <c r="C5" t="s">
-        <v>12</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{87E76E34-AD24-4668-90EA-9119187C3DE2}">
-  <dimension ref="A1:C6"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A15" sqref="A15"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultColWidth="8.77734375" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
-  <cols>
-    <col min="1" max="1" width="24.77734375" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="55.44140625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="35.77734375" bestFit="1" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A1" t="s">
-        <v>0</v>
-      </c>
-      <c r="B1" t="s">
-        <v>1</v>
-      </c>
-      <c r="C1" t="s">
         <v>11</v>
-      </c>
-    </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A2" t="s">
-        <v>14</v>
-      </c>
-      <c r="B2" t="s">
-        <v>2</v>
-      </c>
-      <c r="C2" t="s">
-        <v>13</v>
       </c>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.3">
@@ -591,7 +522,7 @@
         <v>7</v>
       </c>
       <c r="C3" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.3">
@@ -602,7 +533,7 @@
         <v>8</v>
       </c>
       <c r="C4" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.3">
@@ -613,18 +544,7 @@
         <v>9</v>
       </c>
       <c r="C5" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A6" t="s">
-        <v>6</v>
-      </c>
-      <c r="B6" t="s">
-        <v>10</v>
-      </c>
-      <c r="C6" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
     </row>
   </sheetData>

</xml_diff>